<commit_message>
Update to match VSE Export
</commit_message>
<xml_diff>
--- a/VSE_Workloads.xlsx
+++ b/VSE_Workloads.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc6733a6355906f8/Desktop/Code/GO/vse_excel_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc6733a6355906f8/Desktop/Code/GO/vse_excel_import/go_vse_excel_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{E5E41EAA-C010-48C6-8488-2E307F94381C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B6CC8AF-804F-4B42-A812-ABA0A3F3FA30}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{E5E41EAA-C010-48C6-8488-2E307F94381C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D47ABA6D-A9BC-436D-B8A9-07731EACC7B4}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="7395" windowWidth="20610" windowHeight="11970" xr2:uid="{5761B8B4-B076-40BE-87CB-DD9884B8C521}"/>
+    <workbookView xWindow="30345" yWindow="5010" windowWidth="20850" windowHeight="11970" xr2:uid="{5761B8B4-B076-40BE-87CB-DD9884B8C521}"/>
   </bookViews>
   <sheets>
-    <sheet name="workload" sheetId="1" r:id="rId1"/>
+    <sheet name="Workload" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Site</t>
   </si>
@@ -107,19 +107,25 @@
     <t>vm</t>
   </si>
   <si>
-    <t>Window</t>
-  </si>
-  <si>
-    <t>Test_Site</t>
-  </si>
-  <si>
-    <t>Copy_Site</t>
-  </si>
-  <si>
-    <t>myworkload</t>
-  </si>
-  <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Backup Window (hours)</t>
+  </si>
+  <si>
+    <t>Site_A</t>
+  </si>
+  <si>
+    <t>Site_B</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>testWorkload</t>
   </si>
 </sst>
 </file>
@@ -160,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,6 +174,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428BC6EB-2BD7-44B8-972F-4B4B3112F213}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,9 +506,10 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="23" width="16.140625" customWidth="1"/>
     <col min="24" max="24" width="19.28515625" customWidth="1"/>
+    <col min="25" max="25" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,11 +537,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -568,80 +582,90 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="2">
-        <v>287</v>
+        <v>200</v>
       </c>
       <c r="F2" s="2">
-        <v>861</v>
+        <v>600</v>
       </c>
       <c r="G2" s="2">
-        <v>28.12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>5</v>
       </c>
       <c r="I2" s="2">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4">
         <v>3</v>
-      </c>
-      <c r="K2" s="2">
-        <v>8</v>
       </c>
       <c r="L2" s="2">
         <v>50</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="2">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="R2" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="S2" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="T2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U2" s="2">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="V2" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W2" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="X2" s="2">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>